<commit_message>
update structure and generate json files
</commit_message>
<xml_diff>
--- a/data-raw/epu.xlsx
+++ b/data-raw/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="28">
   <si>
     <t>year</t>
   </si>
@@ -87,6 +87,9 @@
     <t>2020</t>
   </si>
   <si>
+    <t>2021</t>
+  </si>
+  <si>
     <t>Source: 'Measuring Economic Policy Uncertainty' by Scott Baker, Nicholas Bloom and Steven J. Davis at www.PolicyUncertainty.com.  These data can be used freely with attribution to the authors, the paper, and the website.</t>
   </si>
   <si>
@@ -137,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C278"/>
+  <dimension ref="A1:C281"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -145,10 +148,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3173,7 +3176,7 @@
         <v>11</v>
       </c>
       <c r="C276" s="0">
-        <v>155.53910827636719</v>
+        <v>214.461669921875</v>
       </c>
     </row>
     <row r="277">
@@ -3184,15 +3187,48 @@
         <v>12</v>
       </c>
       <c r="C277" s="0">
-        <v>177.74766540527344</v>
+        <v>207.60650634765625</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
         <v>24</v>
       </c>
-      <c r="B278" s="0"/>
-      <c r="C278" s="0"/>
+      <c r="B278" s="0">
+        <v>1</v>
+      </c>
+      <c r="C278" s="0">
+        <v>112.63906097412109</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>24</v>
+      </c>
+      <c r="B279" s="0">
+        <v>2</v>
+      </c>
+      <c r="C279" s="0">
+        <v>138.00994873046875</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>24</v>
+      </c>
+      <c r="B280" s="0">
+        <v>3</v>
+      </c>
+      <c r="C280" s="0">
+        <v>141.61357116699219</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>25</v>
+      </c>
+      <c r="B281" s="0"/>
+      <c r="C281" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
create visualization for uk-website
</commit_message>
<xml_diff>
--- a/data-raw/epu.xlsx
+++ b/data-raw/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="28">
   <si>
     <t>year</t>
   </si>
@@ -140,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C281"/>
+  <dimension ref="A1:C282"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -3220,15 +3220,26 @@
         <v>3</v>
       </c>
       <c r="C280" s="0">
-        <v>141.61357116699219</v>
+        <v>140.96719360351562</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
+        <v>24</v>
+      </c>
+      <c r="B281" s="0">
+        <v>4</v>
+      </c>
+      <c r="C281" s="0">
+        <v>89.264839172363281</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
         <v>25</v>
       </c>
-      <c r="B281" s="0"/>
-      <c r="C281" s="0"/>
+      <c r="B282" s="0"/>
+      <c r="C282" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
fix version of psyivx data
</commit_message>
<xml_diff>
--- a/data-raw/epu.xlsx
+++ b/data-raw/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="28">
   <si>
     <t>year</t>
   </si>
@@ -140,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C283"/>
+  <dimension ref="A1:C290"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -3242,15 +3242,92 @@
         <v>5</v>
       </c>
       <c r="C282" s="0">
-        <v>98.790977478027344</v>
+        <v>98.111930847167969</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
+        <v>24</v>
+      </c>
+      <c r="B283" s="0">
+        <v>6</v>
+      </c>
+      <c r="C283" s="0">
+        <v>90.334930419921875</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>24</v>
+      </c>
+      <c r="B284" s="0">
+        <v>7</v>
+      </c>
+      <c r="C284" s="0">
+        <v>88.283767700195313</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>24</v>
+      </c>
+      <c r="B285" s="0">
+        <v>8</v>
+      </c>
+      <c r="C285" s="0">
+        <v>79.109107971191406</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>24</v>
+      </c>
+      <c r="B286" s="0">
+        <v>9</v>
+      </c>
+      <c r="C286" s="0">
+        <v>78.700927734375</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>24</v>
+      </c>
+      <c r="B287" s="0">
+        <v>10</v>
+      </c>
+      <c r="C287" s="0">
+        <v>103.98979187011719</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>24</v>
+      </c>
+      <c r="B288" s="0">
+        <v>11</v>
+      </c>
+      <c r="C288" s="0">
+        <v>75.317497253417969</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>24</v>
+      </c>
+      <c r="B289" s="0">
+        <v>12</v>
+      </c>
+      <c r="C289" s="0">
+        <v>164.3631591796875</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
         <v>25</v>
       </c>
-      <c r="B283" s="0"/>
-      <c r="C283" s="0"/>
+      <c r="B290" s="0"/>
+      <c r="C290" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>